<commit_message>
Stored procedure to find PK keys FindPK_Batch_append_debug.sql
</commit_message>
<xml_diff>
--- a/xls/Dictionary ob objects.xlsx
+++ b/xls/Dictionary ob objects.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esaavedra\Documents\GitHub\SigmaTB_LocalRepo\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B79F0305-1BF9-4D3A-BF34-426293DA28D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFCB5C7-023F-4B43-8A42-4F5586AEB80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{34DB344D-8E49-4CC0-A479-208E1845A7B8}"/>
+    <workbookView xWindow="20760" yWindow="105" windowWidth="17475" windowHeight="15240" activeTab="1" xr2:uid="{34DB344D-8E49-4CC0-A479-208E1845A7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Dic SP" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Dic SP'!$A$1:$C$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>COLUMN</t>
   </si>
@@ -142,14 +145,25 @@
   </si>
   <si>
     <t>CREATION DATE</t>
+  </si>
+  <si>
+    <t>DICTIONARY OF STORED PROCEDURES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -190,10 +204,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,8 +231,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A0EA446-5BF5-4B11-BDF6-7FEF9A1B0C34}" name="Table1" displayName="Table1" ref="A1:C18" totalsRowShown="0">
-  <autoFilter ref="A1:C18" xr:uid="{3A0EA446-5BF5-4B11-BDF6-7FEF9A1B0C34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A0EA446-5BF5-4B11-BDF6-7FEF9A1B0C34}" name="Table1" displayName="Table1" ref="A3:C20" totalsRowShown="0">
+  <autoFilter ref="A3:C20" xr:uid="{3A0EA446-5BF5-4B11-BDF6-7FEF9A1B0C34}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{97B95CD4-A1D6-4B78-864A-BFCB6B7894B4}" name="SCHEMA"/>
     <tableColumn id="2" xr3:uid="{A33D95AC-F184-4BE4-A12C-29A33C7B8BB9}" name="STORED PROCEDURES"/>
@@ -603,10 +618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DD68EC-D6F9-4778-9A0A-FEFE368658B3}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="A1:C18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,36 +632,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45776.312577627315</v>
+      <c r="A1" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45776.293269178241</v>
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,87 +652,87 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2">
-        <v>45776.309978043981</v>
+        <v>45776.312577627315</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
-        <v>45775.74731215278</v>
+        <v>45776.293269178241</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
-        <v>45774.798301655093</v>
+        <v>45776.309978043981</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
-        <v>45774.321174386576</v>
+        <v>45775.74731215278</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2">
-        <v>45774.067171909723</v>
+        <v>45774.798301655093</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>45774.014085185183</v>
+        <v>45774.321174386576</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
-        <v>45769.021399224534</v>
+        <v>45774.067171909723</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>45765.266363888892</v>
+        <v>45774.014085185183</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,10 +740,10 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2">
-        <v>45765.068639583333</v>
+        <v>45769.021399224534</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,10 +751,10 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2">
-        <v>45765.632915509261</v>
+        <v>45765.266363888892</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -764,10 +762,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2">
-        <v>45765.469013541668</v>
+        <v>45765.068639583333</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,10 +773,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2">
-        <v>45765.060139004629</v>
+        <v>45765.632915509261</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -786,10 +784,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2">
-        <v>45764.267441516204</v>
+        <v>45765.469013541668</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -797,10 +795,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2">
-        <v>45764.261846180554</v>
+        <v>45765.060139004629</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,16 +806,39 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45764.267441516204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2">
+        <v>45764.261846180554</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C20" s="2">
         <v>45764.237035300925</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>